<commit_message>
Updated figures, table with germrate analysis, & code
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19455" windowHeight="7680" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19455" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="TABLE1_Rate" sheetId="2" r:id="rId1"/>
@@ -150,7 +150,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -214,118 +234,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor auto="1"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -605,14 +513,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
     <col min="6" max="6" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -644,64 +553,120 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>0.1215</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>0.32219999999999999</v>
+      </c>
+      <c r="E4">
+        <v>0.80940000000000001</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>0.80669999999999997</v>
+      </c>
+      <c r="E5">
+        <v>0.39529999999999998</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>0.21779999999999999</v>
+      </c>
+      <c r="E6">
+        <v>0.88139999999999996</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="E7">
+        <v>0.91090000000000004</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>9.11E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.96289999999999998</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>0.12889999999999999</v>
+      </c>
+      <c r="E9">
+        <v>0.94020000000000004</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -716,64 +681,120 @@
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.1701999999999999</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.30059999999999998</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="B12" s="1">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>12</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.36990000000000001</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.77610000000000001</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3.8300000000000001E-2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.84809999999999997</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="B14" s="1">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.34089999999999998</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.79620000000000002</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>12</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1.1442000000000001</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.30580000000000002</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>12</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1.0106999999999999</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.42180000000000001</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="B17" s="1">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1">
+        <v>12</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1.6957</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.2208</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -788,64 +809,120 @@
       <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>12</v>
+      </c>
+      <c r="D19">
+        <v>0.27239999999999998</v>
+      </c>
+      <c r="E19">
+        <v>0.61119999999999997</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="B20" s="1">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <v>1.5550999999999999</v>
+      </c>
+      <c r="E20">
+        <v>0.25140000000000001</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
+        <v>12</v>
+      </c>
+      <c r="D21">
+        <v>1.8835999999999999</v>
+      </c>
+      <c r="E21">
+        <v>0.19500000000000001</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="B22" s="1">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>12</v>
+      </c>
+      <c r="D22">
+        <v>0.84650000000000003</v>
+      </c>
+      <c r="E22">
+        <v>0.49459999999999998</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>12</v>
+      </c>
+      <c r="D23">
+        <v>2.3740999999999999</v>
+      </c>
+      <c r="E23">
+        <v>0.14929999999999999</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>12</v>
+      </c>
+      <c r="D24">
+        <v>0.37990000000000002</v>
+      </c>
+      <c r="E24">
+        <v>0.76929999999999998</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="B25" s="1">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>12</v>
+      </c>
+      <c r="D25">
+        <v>0.41670000000000001</v>
+      </c>
+      <c r="E25">
+        <v>0.74419999999999997</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -860,64 +937,120 @@
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1">
+        <v>88</v>
+      </c>
+      <c r="D27">
+        <v>2.7199999999999998E-2</v>
+      </c>
+      <c r="E27">
+        <v>0.86939999999999995</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="B28" s="1">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1">
+        <v>88</v>
+      </c>
+      <c r="D28">
+        <v>0.64970000000000006</v>
+      </c>
+      <c r="E28">
+        <v>0.58520000000000005</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1">
+        <v>88</v>
+      </c>
+      <c r="D29">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E29">
+        <v>0.98580000000000001</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="B30" s="1">
+        <v>3</v>
+      </c>
+      <c r="C30" s="1">
+        <v>88</v>
+      </c>
+      <c r="D30">
+        <v>0.22120000000000001</v>
+      </c>
+      <c r="E30">
+        <v>0.88139999999999996</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
+        <v>88</v>
+      </c>
+      <c r="D31">
+        <v>4.2200000000000001E-2</v>
+      </c>
+      <c r="E31">
+        <v>0.83760000000000001</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="B32" s="1">
+        <v>3</v>
+      </c>
+      <c r="C32" s="1">
+        <v>88</v>
+      </c>
+      <c r="D32">
+        <v>0.51129999999999998</v>
+      </c>
+      <c r="E32">
+        <v>0.67549999999999999</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
+      <c r="B33" s="1">
+        <v>3</v>
+      </c>
+      <c r="C33" s="1">
+        <v>88</v>
+      </c>
+      <c r="D33">
+        <v>0.8276</v>
+      </c>
+      <c r="E33">
+        <v>0.48220000000000002</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
@@ -932,64 +1065,120 @@
       <c r="A35" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1">
+        <v>16</v>
+      </c>
+      <c r="D35">
+        <v>2.8574999999999999</v>
+      </c>
+      <c r="E35">
+        <v>0.11033</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
+      <c r="B36" s="1">
+        <v>3</v>
+      </c>
+      <c r="C36" s="1">
+        <v>16</v>
+      </c>
+      <c r="D36">
+        <v>6.1899999999999997E-2</v>
+      </c>
+      <c r="E36">
+        <v>0.97916999999999998</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1">
+        <v>16</v>
+      </c>
+      <c r="D37">
+        <v>6.9665999999999997</v>
+      </c>
+      <c r="E37">
+        <v>1.7850000000000001E-2</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
+      <c r="B38" s="1">
+        <v>3</v>
+      </c>
+      <c r="C38" s="1">
+        <v>16</v>
+      </c>
+      <c r="D38">
+        <v>0.53090000000000004</v>
+      </c>
+      <c r="E38">
+        <v>0.66752</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1">
+        <v>16</v>
+      </c>
+      <c r="D39">
+        <v>2.8574999999999999</v>
+      </c>
+      <c r="E39">
+        <v>0.11033</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
+      <c r="B40" s="1">
+        <v>3</v>
+      </c>
+      <c r="C40" s="1">
+        <v>16</v>
+      </c>
+      <c r="D40">
+        <v>6.1899999999999997E-2</v>
+      </c>
+      <c r="E40">
+        <v>0.97916999999999998</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
+      <c r="B41" s="1">
+        <v>3</v>
+      </c>
+      <c r="C41" s="1">
+        <v>16</v>
+      </c>
+      <c r="D41">
+        <v>0.53090000000000004</v>
+      </c>
+      <c r="E41">
+        <v>0.66752</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
@@ -1004,64 +1193,120 @@
       <c r="A43" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+      <c r="C43" s="1">
+        <v>8</v>
+      </c>
+      <c r="D43">
+        <v>0.1905</v>
+      </c>
+      <c r="E43">
+        <v>0.67410000000000003</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
+      <c r="B44" s="1">
+        <v>3</v>
+      </c>
+      <c r="C44" s="1">
+        <v>8</v>
+      </c>
+      <c r="D44">
+        <v>0.40479999999999999</v>
+      </c>
+      <c r="E44">
+        <v>0.75380000000000003</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
+      <c r="B45" s="1">
+        <v>1</v>
+      </c>
+      <c r="C45" s="1">
+        <v>8</v>
+      </c>
+      <c r="D45">
+        <v>0.21429999999999999</v>
+      </c>
+      <c r="E45">
+        <v>0.65580000000000005</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
+      <c r="B46" s="1">
+        <v>3</v>
+      </c>
+      <c r="C46" s="1">
+        <v>8</v>
+      </c>
+      <c r="D46">
+        <v>1.3332999999999999</v>
+      </c>
+      <c r="E46">
+        <v>0.33</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
+      <c r="B47" s="1">
+        <v>1</v>
+      </c>
+      <c r="C47" s="1">
+        <v>8</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
+      <c r="B48" s="1">
+        <v>3</v>
+      </c>
+      <c r="C48" s="1">
+        <v>8</v>
+      </c>
+      <c r="D48">
+        <v>0.46829999999999999</v>
+      </c>
+      <c r="E48">
+        <v>0.71260000000000001</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
+      <c r="B49" s="1">
+        <v>3</v>
+      </c>
+      <c r="C49" s="1">
+        <v>8</v>
+      </c>
+      <c r="D49">
+        <v>0.88890000000000002</v>
+      </c>
+      <c r="E49">
+        <v>0.48720000000000002</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
@@ -1076,64 +1321,120 @@
       <c r="A51" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
+      <c r="B51" s="1">
+        <v>1</v>
+      </c>
+      <c r="C51" s="1">
+        <v>16</v>
+      </c>
+      <c r="D51">
+        <v>2.0710999999999999</v>
+      </c>
+      <c r="E51">
+        <v>0.1694</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
+      <c r="B52" s="1">
+        <v>3</v>
+      </c>
+      <c r="C52" s="1">
+        <v>16</v>
+      </c>
+      <c r="D52">
+        <v>0.80030000000000001</v>
+      </c>
+      <c r="E52">
+        <v>0.51170000000000004</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
+      <c r="B53" s="1">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1">
+        <v>16</v>
+      </c>
+      <c r="D53">
+        <v>0.80030000000000001</v>
+      </c>
+      <c r="E53">
+        <v>0.38429999999999997</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
+      <c r="B54" s="1">
+        <v>3</v>
+      </c>
+      <c r="C54" s="1">
+        <v>16</v>
+      </c>
+      <c r="D54">
+        <v>0.73980000000000001</v>
+      </c>
+      <c r="E54">
+        <v>0.54369999999999996</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
+      <c r="B55" s="1">
+        <v>1</v>
+      </c>
+      <c r="C55" s="1">
+        <v>16</v>
+      </c>
+      <c r="D55">
+        <v>0.18310000000000001</v>
+      </c>
+      <c r="E55">
+        <v>0.67449999999999999</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
+      <c r="B56" s="1">
+        <v>3</v>
+      </c>
+      <c r="C56" s="1">
+        <v>16</v>
+      </c>
+      <c r="D56">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="E56">
+        <v>0.66549999999999998</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
+      <c r="B57" s="1">
+        <v>3</v>
+      </c>
+      <c r="C57" s="1">
+        <v>16</v>
+      </c>
+      <c r="D57">
+        <v>0.83660000000000001</v>
+      </c>
+      <c r="E57">
+        <v>0.49330000000000002</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C60" s="1"/>
@@ -2105,11 +2406,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="between">
       <formula>0.0499999</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="between">
       <formula>0.04999999</formula>
       <formula>1</formula>
     </cfRule>
@@ -2117,13 +2418,13 @@
       <formula>0.04999999999</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="between">
       <formula>0.0499999</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E59 E70:E1048576">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThan">
       <formula>0.04999999999999</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2136,7 +2437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
@@ -3073,16 +3374,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E59 E70:E1048576">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
       <formula>0.04999999999999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="between">
       <formula>0.0499999</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
       <formula>0.04999999</formula>
       <formula>1</formula>
     </cfRule>
@@ -3090,7 +3391,7 @@
       <formula>0.04999999999</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="between">
       <formula>0.0499999</formula>
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated figures & code
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19455" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19455" windowHeight="7680" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TABLE1_Rate" sheetId="2" r:id="rId1"/>
@@ -52,12 +52,6 @@
     <t>Plantago major</t>
   </si>
   <si>
-    <t>Den DF</t>
-  </si>
-  <si>
-    <t>Num DF</t>
-  </si>
-  <si>
     <t>F-value</t>
   </si>
   <si>
@@ -84,12 +78,18 @@
   <si>
     <t>temp × strat</t>
   </si>
+  <si>
+    <t>Numerator  DF</t>
+  </si>
+  <si>
+    <t>Denominator DF</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +100,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,20 +143,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="36">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -163,6 +170,28 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor auto="1"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -170,6 +199,188 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor auto="1"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor auto="1"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor auto="1"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor auto="1"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor auto="1"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor auto="1"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -513,31 +724,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -602,7 +813,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -619,7 +830,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -636,7 +847,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -653,7 +864,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -730,7 +941,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>3</v>
@@ -747,7 +958,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -764,7 +975,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1">
         <v>3</v>
@@ -781,7 +992,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" s="1">
         <v>3</v>
@@ -858,7 +1069,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B22" s="1">
         <v>3</v>
@@ -875,7 +1086,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
@@ -892,7 +1103,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B24" s="1">
         <v>3</v>
@@ -909,7 +1120,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B25" s="1">
         <v>3</v>
@@ -986,7 +1197,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B30" s="1">
         <v>3</v>
@@ -1003,7 +1214,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B31" s="1">
         <v>1</v>
@@ -1020,7 +1231,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B32" s="1">
         <v>3</v>
@@ -1037,7 +1248,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B33" s="1">
         <v>3</v>
@@ -1114,7 +1325,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B38" s="1">
         <v>3</v>
@@ -1131,7 +1342,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B39" s="1">
         <v>1</v>
@@ -1148,7 +1359,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B40" s="1">
         <v>3</v>
@@ -1165,7 +1376,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B41" s="1">
         <v>3</v>
@@ -1182,7 +1393,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1242,7 +1453,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B46" s="1">
         <v>3</v>
@@ -1259,7 +1470,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B47" s="1">
         <v>1</v>
@@ -1276,7 +1487,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B48" s="1">
         <v>3</v>
@@ -1293,7 +1504,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B49" s="1">
         <v>3</v>
@@ -1310,7 +1521,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -1370,7 +1581,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B54" s="1">
         <v>3</v>
@@ -1387,7 +1598,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B55" s="1">
         <v>1</v>
@@ -1404,7 +1615,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B56" s="1">
         <v>3</v>
@@ -1421,7 +1632,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B57" s="1">
         <v>3</v>
@@ -1467,6 +1678,29 @@
       <c r="E65" s="1"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E1">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="greaterThan">
+      <formula>0.04999999999999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="between">
+      <formula>0.0499999</formula>
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="between">
+      <formula>0.04999999</formula>
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="between">
+      <formula>0.04999999999</formula>
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="between">
+      <formula>0.0499999</formula>
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1476,30 +1710,31 @@
   <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="7"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1509,7 +1744,7 @@
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="5"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1524,7 +1759,7 @@
       <c r="D3" s="1">
         <v>0.27715000000000001</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>0.6915</v>
       </c>
     </row>
@@ -1541,7 +1776,7 @@
       <c r="D4" s="1">
         <v>1.49902</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>0.2359</v>
       </c>
     </row>
@@ -1558,13 +1793,13 @@
       <c r="D5" s="1">
         <v>0.43162</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>0.5151</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
@@ -1575,13 +1810,13 @@
       <c r="D6" s="1">
         <v>1.0025200000000001</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>0.37619999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -1592,13 +1827,13 @@
       <c r="D7" s="1">
         <v>1.8950000000000002E-2</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>0.89119999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
@@ -1609,13 +1844,13 @@
       <c r="D8" s="1">
         <v>1.6620999999999999</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>0.2029</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
@@ -1626,7 +1861,7 @@
       <c r="D9" s="1">
         <v>1.24546</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>0.29899999999999999</v>
       </c>
     </row>
@@ -1637,7 +1872,7 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="5"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1652,7 +1887,7 @@
       <c r="D11" s="1">
         <v>10.928000000000001</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="8">
         <v>8.0600000000000005E-2</v>
       </c>
     </row>
@@ -1669,8 +1904,8 @@
       <c r="D12" s="1">
         <v>27.422000000000001</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>14</v>
+      <c r="E12" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1686,13 +1921,13 @@
       <c r="D13" s="1">
         <v>0.59099999999999997</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="8">
         <v>0.44400000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>3</v>
@@ -1703,13 +1938,13 @@
       <c r="D14" s="1">
         <v>2.9319999999999999</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="8">
         <v>3.7499999999999999E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -1720,13 +1955,13 @@
       <c r="D15" s="1">
         <v>4.6609999999999996</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="8">
         <v>3.3399999999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1">
         <v>3</v>
@@ -1737,13 +1972,13 @@
       <c r="D16" s="1">
         <v>2.6379999999999999</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="8">
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" s="1">
         <v>3</v>
@@ -1754,7 +1989,7 @@
       <c r="D17" s="1">
         <v>1.0640000000000001</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="8">
         <v>0.36840000000000001</v>
       </c>
     </row>
@@ -1765,7 +2000,7 @@
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="5"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
@@ -1780,7 +2015,7 @@
       <c r="D19">
         <v>0.11559999999999999</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="8">
         <v>0.76619999999999999</v>
       </c>
     </row>
@@ -1797,7 +2032,7 @@
       <c r="D20">
         <v>7.5346000000000002</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="8">
         <v>1E-4</v>
       </c>
     </row>
@@ -1814,13 +2049,13 @@
       <c r="D21">
         <v>2.9228999999999998</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="8">
         <v>9.0700000000000003E-2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -1831,13 +2066,13 @@
       <c r="D22">
         <v>1.7851999999999999</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="8">
         <v>0.1555</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1848,13 +2083,13 @@
       <c r="D23">
         <v>6.3769999999999998</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="8">
         <v>1.3299999999999999E-2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -1865,13 +2100,13 @@
       <c r="D24">
         <v>0.4909</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="8">
         <v>0.68940000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -1882,7 +2117,7 @@
       <c r="D25">
         <v>0.4783</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="8">
         <v>0.69810000000000005</v>
       </c>
     </row>
@@ -1893,7 +2128,7 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="5"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -1908,7 +2143,7 @@
       <c r="D27">
         <v>0.21310000000000001</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="8">
         <v>0.65339999999999998</v>
       </c>
     </row>
@@ -1925,8 +2160,8 @@
       <c r="D28">
         <v>41.258099999999999</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>14</v>
+      <c r="E28" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1942,13 +2177,13 @@
       <c r="D29">
         <v>17.845400000000001</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>14</v>
+      <c r="E29" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -1959,13 +2194,13 @@
       <c r="D30">
         <v>2.6467999999999998</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="8">
         <v>4.87E-2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1976,13 +2211,13 @@
       <c r="D31">
         <v>5.2499999999999998E-2</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="8">
         <v>0.81889999999999996</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -1993,13 +2228,13 @@
       <c r="D32">
         <v>2.8193999999999999</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="8">
         <v>3.8800000000000001E-2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B33">
         <v>3</v>
@@ -2010,7 +2245,7 @@
       <c r="D33">
         <v>6.9433999999999996</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="8">
         <v>1E-4</v>
       </c>
     </row>
@@ -2021,7 +2256,7 @@
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
-      <c r="E34" s="5"/>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
@@ -2036,7 +2271,7 @@
       <c r="D35" s="1">
         <v>2.2012</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="5">
         <v>0.2762</v>
       </c>
     </row>
@@ -2053,8 +2288,8 @@
       <c r="D36" s="1">
         <v>30.2088</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>14</v>
+      <c r="E36" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2070,13 +2305,13 @@
       <c r="D37" s="1">
         <v>1.5368999999999999</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="5">
         <v>0.21729999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B38" s="1">
         <v>3</v>
@@ -2087,13 +2322,13 @@
       <c r="D38" s="1">
         <v>0.73750000000000004</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="5">
         <v>0.53149999999999997</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B39" s="1">
         <v>1</v>
@@ -2104,13 +2339,13 @@
       <c r="D39" s="1">
         <v>7.1170999999999998</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="5">
         <v>8.6E-3</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B40" s="1">
         <v>3</v>
@@ -2121,13 +2356,13 @@
       <c r="D40" s="1">
         <v>0.75970000000000004</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="5">
         <v>0.51870000000000005</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B41" s="1">
         <v>3</v>
@@ -2138,18 +2373,18 @@
       <c r="D41" s="1">
         <v>1.5258</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="5">
         <v>0.21079999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
-      <c r="E42" s="5"/>
+      <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
@@ -2164,7 +2399,7 @@
       <c r="D43" s="1">
         <v>12.083500000000001</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="5">
         <v>0.17829999999999999</v>
       </c>
     </row>
@@ -2181,8 +2416,8 @@
       <c r="D44" s="1">
         <v>9.3773</v>
       </c>
-      <c r="E44" s="6" t="s">
-        <v>14</v>
+      <c r="E44" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2198,13 +2433,13 @@
       <c r="D45" s="1">
         <v>0.1132</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45" s="5">
         <v>0.73709999999999998</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B46" s="1">
         <v>3</v>
@@ -2215,13 +2450,13 @@
       <c r="D46" s="1">
         <v>3.2383999999999999</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46" s="5">
         <v>2.4400000000000002E-2</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B47" s="1">
         <v>1</v>
@@ -2232,13 +2467,13 @@
       <c r="D47" s="1">
         <v>41.0184</v>
       </c>
-      <c r="E47" s="6" t="s">
-        <v>14</v>
+      <c r="E47" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B48" s="1">
         <v>3</v>
@@ -2249,13 +2484,13 @@
       <c r="D48" s="1">
         <v>1.5444</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="5">
         <v>0.20610000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B49" s="1">
         <v>3</v>
@@ -2266,18 +2501,18 @@
       <c r="D49" s="1">
         <v>2.1785999999999999</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E49" s="5">
         <v>9.3600000000000003E-2</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
-      <c r="E50" s="5"/>
+      <c r="E50" s="7"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
@@ -2292,7 +2527,7 @@
       <c r="D51" s="1">
         <v>5.3860000000000001</v>
       </c>
-      <c r="E51" s="7">
+      <c r="E51" s="8">
         <v>0.14599999999999999</v>
       </c>
     </row>
@@ -2309,7 +2544,7 @@
       <c r="D52" s="1">
         <v>3.6469999999999998</v>
       </c>
-      <c r="E52" s="7">
+      <c r="E52" s="8">
         <v>1.47E-2</v>
       </c>
     </row>
@@ -2326,13 +2561,13 @@
       <c r="D53" s="1">
         <v>9.4390000000000001</v>
       </c>
-      <c r="E53" s="7">
+      <c r="E53" s="8">
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B54" s="1">
         <v>3</v>
@@ -2343,13 +2578,13 @@
       <c r="D54" s="1">
         <v>1.597</v>
       </c>
-      <c r="E54" s="7">
+      <c r="E54" s="8">
         <v>0.19359999999999999</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B55" s="1">
         <v>1</v>
@@ -2360,13 +2595,13 @@
       <c r="D55" s="1">
         <v>36.344000000000001</v>
       </c>
-      <c r="E55" s="7" t="s">
-        <v>14</v>
+      <c r="E55" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B56" s="1">
         <v>3</v>
@@ -2377,13 +2612,13 @@
       <c r="D56" s="1">
         <v>0.41399999999999998</v>
       </c>
-      <c r="E56" s="7">
+      <c r="E56" s="8">
         <v>0.74309999999999998</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B57" s="1">
         <v>3</v>
@@ -2394,40 +2629,17 @@
       <c r="D57" s="1">
         <v>2.2410000000000001</v>
       </c>
-      <c r="E57" s="7">
+      <c r="E57" s="8">
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E58" s="6"/>
+      <c r="E58" s="5"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E59" s="6"/>
+      <c r="E59" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="between">
-      <formula>0.0499999</formula>
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="between">
-      <formula>0.04999999</formula>
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="3" operator="between">
-      <formula>0.04999999999</formula>
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="between">
-      <formula>0.0499999</formula>
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E59 E70:E1048576">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThan">
-      <formula>0.04999999999999</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
@@ -2437,31 +2649,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="7"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2471,7 +2683,7 @@
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="5"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2486,7 +2698,7 @@
       <c r="D3" s="1">
         <v>0.49363000000000001</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>0.61009999999999998</v>
       </c>
     </row>
@@ -2503,7 +2715,7 @@
       <c r="D4" s="1">
         <v>26.451889999999999</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>1E-4</v>
       </c>
     </row>
@@ -2520,13 +2732,13 @@
       <c r="D5" s="1">
         <v>9.1686499999999995</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -2537,13 +2749,13 @@
       <c r="D6" s="1">
         <v>6.9718099999999996</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>1.61E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -2554,13 +2766,13 @@
       <c r="D7" s="1">
         <v>3.6422300000000001</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>7.1599999999999997E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -2571,13 +2783,13 @@
       <c r="D8" s="1">
         <v>0.44191000000000003</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>0.51419999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -2588,7 +2800,7 @@
       <c r="D9" s="1">
         <v>6.89595</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>1.66E-2</v>
       </c>
     </row>
@@ -2599,7 +2811,7 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="5"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -2614,7 +2826,7 @@
       <c r="D11">
         <v>49.023899999999998</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="8">
         <v>1.9800000000000002E-2</v>
       </c>
     </row>
@@ -2631,8 +2843,8 @@
       <c r="D12">
         <v>42.369399999999999</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>14</v>
+      <c r="E12" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2648,13 +2860,13 @@
       <c r="D13">
         <v>4.9397000000000002</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="8">
         <v>2.98E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -2665,13 +2877,13 @@
       <c r="D14">
         <v>0.61960000000000004</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="8">
         <v>0.54139999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2682,13 +2894,13 @@
       <c r="D15">
         <v>40.9529</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>14</v>
+      <c r="E15" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -2699,13 +2911,13 @@
       <c r="D16">
         <v>7.0194000000000001</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="8">
         <v>1.8E-3</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -2716,8 +2928,8 @@
       <c r="D17">
         <v>17.513500000000001</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>14</v>
+      <c r="E17" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2727,7 +2939,7 @@
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="5"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
@@ -2742,7 +2954,7 @@
       <c r="D19">
         <v>0</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="8">
         <v>0.998</v>
       </c>
     </row>
@@ -2759,8 +2971,8 @@
       <c r="D20">
         <v>26.9803</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>14</v>
+      <c r="E20" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2776,13 +2988,13 @@
       <c r="D21">
         <v>1.3894</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="8">
         <v>0.2417</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -2793,13 +3005,13 @@
       <c r="D22">
         <v>3.0743999999999998</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="8">
         <v>3.1699999999999999E-2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -2810,13 +3022,13 @@
       <c r="D23">
         <v>2.1835</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="8">
         <v>0.14299999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -2827,13 +3039,13 @@
       <c r="D24">
         <v>1.6354</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="8">
         <v>0.18690000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -2844,7 +3056,7 @@
       <c r="D25">
         <v>1.1286</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="8">
         <v>0.34189999999999998</v>
       </c>
     </row>
@@ -2855,7 +3067,7 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="5"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -2870,7 +3082,7 @@
       <c r="D27">
         <v>4.5199999999999997E-2</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="8">
         <v>0.83550000000000002</v>
       </c>
     </row>
@@ -2887,8 +3099,8 @@
       <c r="D28">
         <v>62.520699999999998</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>14</v>
+      <c r="E28" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2904,13 +3116,13 @@
       <c r="D29">
         <v>1.0047999999999999</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="8">
         <v>0.31680000000000003</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -2921,13 +3133,13 @@
       <c r="D30">
         <v>12.7363</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>14</v>
+      <c r="E30" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -2938,13 +3150,13 @@
       <c r="D31">
         <v>2.1457000000000002</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="8">
         <v>0.14380000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -2955,13 +3167,13 @@
       <c r="D32">
         <v>0.65559999999999996</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="8">
         <v>0.57989999999999997</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B33">
         <v>3</v>
@@ -2972,7 +3184,7 @@
       <c r="D33">
         <v>2.1232000000000002</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="8">
         <v>9.6799999999999997E-2</v>
       </c>
     </row>
@@ -2983,7 +3195,7 @@
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
-      <c r="E34" s="5"/>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
@@ -2998,7 +3210,7 @@
       <c r="D35" s="1">
         <v>0.63614999999999999</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="5">
         <v>0.50880000000000003</v>
       </c>
     </row>
@@ -3015,8 +3227,8 @@
       <c r="D36" s="1">
         <v>92.350239999999999</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>14</v>
+      <c r="E36" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3032,13 +3244,13 @@
       <c r="D37" s="1">
         <v>111.84332000000001</v>
       </c>
-      <c r="E37" s="6" t="s">
-        <v>14</v>
+      <c r="E37" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B38" s="1">
         <v>3</v>
@@ -3049,13 +3261,13 @@
       <c r="D38" s="1">
         <v>3.3337699999999999</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="5">
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B39" s="1">
         <v>1</v>
@@ -3066,13 +3278,13 @@
       <c r="D39" s="1">
         <v>9.6512600000000006</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="5">
         <v>2.3E-3</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B40" s="1">
         <v>3</v>
@@ -3083,13 +3295,13 @@
       <c r="D40" s="1">
         <v>44.822209999999998</v>
       </c>
-      <c r="E40" s="6" t="s">
-        <v>14</v>
+      <c r="E40" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B41" s="1">
         <v>3</v>
@@ -3100,18 +3312,18 @@
       <c r="D41" s="1">
         <v>0.60326000000000002</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="5">
         <v>0.61399999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
-      <c r="E42" s="5"/>
+      <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
@@ -3126,7 +3338,7 @@
       <c r="D43" s="1">
         <v>7.5935300000000003</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="5">
         <v>0.22159999999999999</v>
       </c>
     </row>
@@ -3143,8 +3355,8 @@
       <c r="D44" s="1">
         <v>141.50366</v>
       </c>
-      <c r="E44" s="6" t="s">
-        <v>14</v>
+      <c r="E44" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3160,13 +3372,13 @@
       <c r="D45" s="1">
         <v>5.2366299999999999</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45" s="5">
         <v>2.3800000000000002E-2</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B46" s="1">
         <v>3</v>
@@ -3177,13 +3389,13 @@
       <c r="D46" s="1">
         <v>17.07808</v>
       </c>
-      <c r="E46" s="6" t="s">
-        <v>14</v>
+      <c r="E46" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B47" s="1">
         <v>1</v>
@@ -3194,13 +3406,13 @@
       <c r="D47" s="1">
         <v>17.380649999999999</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="5">
         <v>1E-4</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B48" s="1">
         <v>3</v>
@@ -3211,13 +3423,13 @@
       <c r="D48" s="1">
         <v>4.7558600000000002</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="5">
         <v>3.5999999999999999E-3</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B49" s="1">
         <v>3</v>
@@ -3228,18 +3440,18 @@
       <c r="D49" s="1">
         <v>12.16155</v>
       </c>
-      <c r="E49" s="6" t="s">
-        <v>14</v>
+      <c r="E49" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
-      <c r="E50" s="5"/>
+      <c r="E50" s="7"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
@@ -3254,7 +3466,7 @@
       <c r="D51">
         <v>0.13619999999999999</v>
       </c>
-      <c r="E51" s="7">
+      <c r="E51" s="8">
         <v>0.74750000000000005</v>
       </c>
     </row>
@@ -3271,8 +3483,8 @@
       <c r="D52">
         <v>11.98401</v>
       </c>
-      <c r="E52" s="7" t="s">
-        <v>14</v>
+      <c r="E52" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3288,13 +3500,13 @@
       <c r="D53">
         <v>16.481030000000001</v>
       </c>
-      <c r="E53" s="7">
+      <c r="E53" s="8">
         <v>1E-4</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B54">
         <v>3</v>
@@ -3305,13 +3517,13 @@
       <c r="D54">
         <v>0.33156999999999998</v>
       </c>
-      <c r="E54" s="7">
+      <c r="E54" s="8">
         <v>0.80249999999999999</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -3322,13 +3534,13 @@
       <c r="D55">
         <v>3.2202500000000001</v>
       </c>
-      <c r="E55" s="7">
+      <c r="E55" s="8">
         <v>7.5399999999999995E-2</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B56">
         <v>3</v>
@@ -3339,13 +3551,13 @@
       <c r="D56">
         <v>3.1975600000000002</v>
       </c>
-      <c r="E56" s="7">
+      <c r="E56" s="8">
         <v>2.6100000000000002E-2</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B57">
         <v>3</v>
@@ -3356,7 +3568,7 @@
       <c r="D57">
         <v>3.2147600000000001</v>
       </c>
-      <c r="E57" s="7">
+      <c r="E57" s="8">
         <v>2.5499999999999998E-2</v>
       </c>
     </row>
@@ -3364,38 +3576,15 @@
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
-      <c r="E58" s="6"/>
+      <c r="E58" s="5"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
-      <c r="E59" s="6"/>
+      <c r="E59" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:E59 E70:E1048576">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
-      <formula>0.04999999999999</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="between">
-      <formula>0.0499999</formula>
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
-      <formula>0.04999999</formula>
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="3" operator="between">
-      <formula>0.04999999999</formula>
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="between">
-      <formula>0.0499999</formula>
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>